<commit_message>
SPR-3078 [jylee_fix] add web.module.ts export whole services, excel export channel type change view -> View, add pdview_index on excel export logic
</commit_message>
<xml_diff>
--- a/src/database/seeds/IMS_CAMERA_GROUP_INFO_ADD_SKELETON.xlsx
+++ b/src/database/seeds/IMS_CAMERA_GROUP_INFO_ADD_SKELETON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\var\www\code\ims_be_v2\src\database\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2FC1F6-7CC0-48FF-9D41-56765A52850F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653F4E2A-C5E7-46CE-AAB2-200EFC9F57EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A567769-202B-469D-BB8A-3227741A9574}"/>
   </bookViews>
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="252">
   <si>
     <t>IMS system_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1096,6 +1096,42 @@
     <t>channel index</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>MULTIVIEWA-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTIVIEWB-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTIVIEWC-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTIVIEWD-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTIVIEWE-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MULTIVIEWF-AUDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRAVIEWA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRAVIEWB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXTRAVIEWC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1491,7 +1527,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1573,14 +1609,8 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="3" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1591,11 +1621,20 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1641,6 +1680,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -30355,9 +30397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CFCB73-D077-4A92-8EA6-305BED3F48DA}">
   <dimension ref="A1:AX103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AX12" sqref="AX12"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.5" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -30403,17 +30445,17 @@
       <c r="H1" s="33"/>
       <c r="I1" s="33"/>
       <c r="J1" s="33"/>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="29"/>
       <c r="Q1" s="24"/>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="51"/>
+      <c r="S1" s="51" t="s">
         <v>237</v>
       </c>
-      <c r="S1" s="29"/>
       <c r="T1" s="25"/>
       <c r="U1" s="26"/>
     </row>
@@ -30428,16 +30470,16 @@
       <c r="H2" s="33"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="R2" s="29" t="s">
+      <c r="M2" s="35"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51" t="s">
         <v>236</v>
       </c>
-      <c r="S2" s="29"/>
       <c r="U2" s="26"/>
     </row>
     <row r="3" spans="1:50" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -30552,10 +30594,10 @@
       <c r="AR9" s="34"/>
       <c r="AS9" s="34"/>
       <c r="AT9" s="34"/>
-      <c r="AV9" s="27" t="s">
+      <c r="AV9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AX9" s="27" t="s">
+      <c r="AX9" s="31" t="s">
         <v>240</v>
       </c>
     </row>
@@ -30611,8 +30653,8 @@
       <c r="AR10" s="34"/>
       <c r="AS10" s="34"/>
       <c r="AT10" s="34"/>
-      <c r="AV10" s="28"/>
-      <c r="AX10" s="28"/>
+      <c r="AV10" s="32"/>
+      <c r="AX10" s="32"/>
     </row>
     <row r="11" spans="1:50" s="15" customFormat="1" ht="126.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
@@ -35091,7 +35133,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="15">
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="AX9:AX10"/>
     <mergeCell ref="A1:J7"/>
     <mergeCell ref="L9:X10"/>
@@ -35102,13 +35147,8 @@
     <mergeCell ref="Z10:AE10"/>
     <mergeCell ref="AF10:AK10"/>
     <mergeCell ref="Z9:AK9"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="R1:S1"/>
     <mergeCell ref="AV9:AV10"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="Y18:AT18 J14:AT14 J16:AT16 J17:L17 J18:T18 J15:S15 R17:S17 J29:K29 Y22:AT22 J20:AT20 J21:L21 J19:S19 R21:S21 T26:AT28 J24:S28 A97:AT103 J33:AT33 J34:AE35 AG34:AL34 Y13:AE13 AG13:AL13 K23:N23 P23 P13:T13 U24:AT24 Y23 T32:AE32 AG32:AH32 AJ32:AT32 J32:S34 J22:T22 L23:N24 AF21:AK22 J30:AT31 I23:J31 AV97:AV103 B92 AV53:AV94 B94 D53:G94 I53:AT91 I92:N94 P92:S92 P93:P94 R93:S93 S94 R94:R96 Y92:Y94 AL92:AL94 I13:N13 J32:L41 M33:T41 Y36:AE41 AJ35:AL41 K39:M41 I43:AT51 AG35:AH41 I40:AE41 A13:A41 C13:G41 J13:J51 I13:I41 AM34:AT41 J42:N42 I43:I96 D43:G51 G43:G96 E43:E95 C43:D96 A43:A96 AV13:AV51">
@@ -51407,7 +51447,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX13">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="133" priority="1">
       <formula>$L13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51433,10 +51473,10 @@
       <formula1>"모노,스테레오,서라운드"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P13:P103" xr:uid="{1D963593-3F91-4BB2-91BE-1C09F314379D}">
-      <formula1>"MainView,SubView"</formula1>
+      <formula1>"MainView,SubView,ExtraView"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M13:M103" xr:uid="{1020EDE3-B039-46A8-A236-B38BA346394B}">
-      <formula1>"MAINVIEW,MULTIVIEW,BIRDVIEW,EXTERNAL,PDVIEW"</formula1>
+      <formula1>"MAINVIEW,MULTIVIEW,BIRDVIEW,EXTERNAL,PDVIEW,EXTRAVIEW"</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R13:S103" xr:uid="{B29A248C-0415-4881-8267-2A544D117E94}">
       <formula1>0</formula1>
@@ -51455,7 +51495,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{070DD72D-54D1-4657-93AD-AE5552A89DA3}">
           <x14:formula1>
-            <xm:f>코드!$A$1:$A$29</xm:f>
+            <xm:f>코드!$A$1:$A$40</xm:f>
           </x14:formula1>
           <xm:sqref>N13:N103</xm:sqref>
         </x14:dataValidation>
@@ -51482,143 +51522,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
     </row>
     <row r="9" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="38"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
@@ -53729,302 +53769,302 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N61:N64 N66:N69 K14:N14 N15 L16:N18 M80:N82 L78:N79 K78:K83 N45 N28:N32 N71:N74 N77 K28:M28 L30:M32 I31:J31 K47:M47 L49:N51 I50:J50 K61:M61 L63:M65 I64:J64 K67:M67 L69:M71 I70:J70 K73:M73 L75:M77 I76:J76 A84:N145 A52:N59 A13:N13 A30:J30 A28:H28 A46:M46 A49:J49 A47:H47 A60:M60 A63:J63 A61:H61 A66:M66 A69:J69 A67:H67 A72:M72 A75:J75 A73:H73 A78:J82 A83:B83 A33:N44 A45:J45 A25:M27 A29:G29 A31:H32 A48:G48 A50:H51 A62:G62 A64:H65 A68:G68 A70:H71 A74:G74 A76:H77 N19:N25 I16:J17 A14:H18">
-    <cfRule type="expression" dxfId="133" priority="618">
+    <cfRule type="expression" dxfId="132" priority="618">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N26">
-    <cfRule type="expression" dxfId="132" priority="525">
+    <cfRule type="expression" dxfId="131" priority="525">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L82">
-    <cfRule type="expression" dxfId="131" priority="519">
+    <cfRule type="expression" dxfId="130" priority="519">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L81">
-    <cfRule type="expression" dxfId="130" priority="517">
+    <cfRule type="expression" dxfId="129" priority="517">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L80">
-    <cfRule type="expression" dxfId="129" priority="515">
+    <cfRule type="expression" dxfId="128" priority="515">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N76">
-    <cfRule type="expression" dxfId="128" priority="511">
+    <cfRule type="expression" dxfId="127" priority="511">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N75">
-    <cfRule type="expression" dxfId="127" priority="510">
+    <cfRule type="expression" dxfId="126" priority="510">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N70">
-    <cfRule type="expression" dxfId="126" priority="509">
+    <cfRule type="expression" dxfId="125" priority="509">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N65">
-    <cfRule type="expression" dxfId="125" priority="508">
+    <cfRule type="expression" dxfId="124" priority="508">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N60">
-    <cfRule type="expression" dxfId="124" priority="507">
+    <cfRule type="expression" dxfId="123" priority="507">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="expression" dxfId="123" priority="506">
+    <cfRule type="expression" dxfId="122" priority="506">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N83">
-    <cfRule type="expression" dxfId="122" priority="505">
+    <cfRule type="expression" dxfId="121" priority="505">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L83">
-    <cfRule type="expression" dxfId="121" priority="502">
+    <cfRule type="expression" dxfId="120" priority="502">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H83">
-    <cfRule type="expression" dxfId="120" priority="504">
+    <cfRule type="expression" dxfId="119" priority="504">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I83:J83">
-    <cfRule type="expression" dxfId="119" priority="503">
+    <cfRule type="expression" dxfId="118" priority="503">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83">
-    <cfRule type="expression" dxfId="118" priority="501">
+    <cfRule type="expression" dxfId="117" priority="501">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:E83">
-    <cfRule type="expression" dxfId="117" priority="499">
+    <cfRule type="expression" dxfId="116" priority="499">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83">
-    <cfRule type="expression" dxfId="116" priority="498">
+    <cfRule type="expression" dxfId="115" priority="498">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83">
-    <cfRule type="expression" dxfId="115" priority="497">
+    <cfRule type="expression" dxfId="114" priority="497">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:M15">
-    <cfRule type="expression" dxfId="114" priority="496">
+    <cfRule type="expression" dxfId="113" priority="496">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:K17">
-    <cfRule type="expression" dxfId="113" priority="495">
+    <cfRule type="expression" dxfId="112" priority="495">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="112" priority="494">
+    <cfRule type="expression" dxfId="111" priority="494">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:J14">
-    <cfRule type="expression" dxfId="111" priority="493">
+    <cfRule type="expression" dxfId="110" priority="493">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:J18">
-    <cfRule type="expression" dxfId="110" priority="492">
+    <cfRule type="expression" dxfId="109" priority="492">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:M45">
-    <cfRule type="expression" dxfId="109" priority="467">
+    <cfRule type="expression" dxfId="108" priority="467">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46">
-    <cfRule type="expression" dxfId="108" priority="461">
+    <cfRule type="expression" dxfId="107" priority="461">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N47">
-    <cfRule type="expression" dxfId="107" priority="455">
+    <cfRule type="expression" dxfId="106" priority="455">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="expression" dxfId="106" priority="449">
+    <cfRule type="expression" dxfId="105" priority="449">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:M29">
-    <cfRule type="expression" dxfId="105" priority="364">
+    <cfRule type="expression" dxfId="104" priority="364">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:K31">
-    <cfRule type="expression" dxfId="104" priority="363">
+    <cfRule type="expression" dxfId="103" priority="363">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="expression" dxfId="103" priority="362">
+    <cfRule type="expression" dxfId="102" priority="362">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:J28">
-    <cfRule type="expression" dxfId="102" priority="361">
+    <cfRule type="expression" dxfId="101" priority="361">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:J32">
-    <cfRule type="expression" dxfId="101" priority="360">
+    <cfRule type="expression" dxfId="100" priority="360">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48:M48">
-    <cfRule type="expression" dxfId="100" priority="356">
+    <cfRule type="expression" dxfId="99" priority="356">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K50">
-    <cfRule type="expression" dxfId="99" priority="355">
+    <cfRule type="expression" dxfId="98" priority="355">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51">
-    <cfRule type="expression" dxfId="98" priority="354">
+    <cfRule type="expression" dxfId="97" priority="354">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:J47">
-    <cfRule type="expression" dxfId="97" priority="353">
+    <cfRule type="expression" dxfId="96" priority="353">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I51:J51">
-    <cfRule type="expression" dxfId="96" priority="352">
+    <cfRule type="expression" dxfId="95" priority="352">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62:M62">
-    <cfRule type="expression" dxfId="95" priority="303">
+    <cfRule type="expression" dxfId="94" priority="303">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:K64">
-    <cfRule type="expression" dxfId="94" priority="302">
+    <cfRule type="expression" dxfId="93" priority="302">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K65">
-    <cfRule type="expression" dxfId="93" priority="301">
+    <cfRule type="expression" dxfId="92" priority="301">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:J61">
-    <cfRule type="expression" dxfId="92" priority="300">
+    <cfRule type="expression" dxfId="91" priority="300">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65:J65">
-    <cfRule type="expression" dxfId="91" priority="299">
+    <cfRule type="expression" dxfId="90" priority="299">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:M68">
-    <cfRule type="expression" dxfId="90" priority="214">
+    <cfRule type="expression" dxfId="89" priority="214">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69:K70">
-    <cfRule type="expression" dxfId="89" priority="213">
+    <cfRule type="expression" dxfId="88" priority="213">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71">
-    <cfRule type="expression" dxfId="88" priority="212">
+    <cfRule type="expression" dxfId="87" priority="212">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67:J67">
-    <cfRule type="expression" dxfId="87" priority="211">
+    <cfRule type="expression" dxfId="86" priority="211">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I71:J71">
-    <cfRule type="expression" dxfId="86" priority="210">
+    <cfRule type="expression" dxfId="85" priority="210">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H74:M74">
-    <cfRule type="expression" dxfId="85" priority="55">
+    <cfRule type="expression" dxfId="84" priority="55">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K75:K76">
-    <cfRule type="expression" dxfId="84" priority="54">
+    <cfRule type="expression" dxfId="83" priority="54">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77">
-    <cfRule type="expression" dxfId="83" priority="53">
+    <cfRule type="expression" dxfId="82" priority="53">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I73:J73">
-    <cfRule type="expression" dxfId="82" priority="52">
+    <cfRule type="expression" dxfId="81" priority="52">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I77:J77">
-    <cfRule type="expression" dxfId="81" priority="51">
+    <cfRule type="expression" dxfId="80" priority="51">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:M20 L22:M24 A19:G24 I19:M19 I22:J23">
-    <cfRule type="expression" dxfId="80" priority="19">
+    <cfRule type="expression" dxfId="79" priority="19">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:M21">
-    <cfRule type="expression" dxfId="79" priority="18">
+    <cfRule type="expression" dxfId="78" priority="18">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:K23">
-    <cfRule type="expression" dxfId="78" priority="17">
+    <cfRule type="expression" dxfId="77" priority="17">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="expression" dxfId="77" priority="16">
+    <cfRule type="expression" dxfId="76" priority="16">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:J20">
-    <cfRule type="expression" dxfId="76" priority="15">
+    <cfRule type="expression" dxfId="75" priority="15">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:J24">
-    <cfRule type="expression" dxfId="75" priority="14">
+    <cfRule type="expression" dxfId="74" priority="14">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19:H24">
-    <cfRule type="expression" dxfId="74" priority="3">
+    <cfRule type="expression" dxfId="73" priority="3">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54129,7 +54169,7 @@
       <c r="AS5" s="34"/>
       <c r="AT5" s="34"/>
       <c r="AU5" s="34"/>
-      <c r="AW5" s="40" t="s">
+      <c r="AW5" s="41" t="s">
         <v>144</v>
       </c>
     </row>
@@ -54185,7 +54225,7 @@
       <c r="AS6" s="34"/>
       <c r="AT6" s="34"/>
       <c r="AU6" s="34"/>
-      <c r="AW6" s="28"/>
+      <c r="AW6" s="32"/>
     </row>
     <row r="7" spans="2:49" ht="54" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -56336,367 +56376,367 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="AW29:AW32 B8:H28 AJ29:AJ32 J29:AI29 AK29:AU29 K9:K28">
-    <cfRule type="expression" dxfId="73" priority="1">
+    <cfRule type="expression" dxfId="72" priority="1">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31:AI32 AK31:AU32 AW8:AW28 J30:M30 B29:H32">
-    <cfRule type="expression" dxfId="72" priority="73">
+    <cfRule type="expression" dxfId="71" priority="73">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:U24 Z8:AU24 S30:T30 I8:O8 L24 L25:AU25 I24:K25 I9:L23 M9:O24 J31:U32 I26:AU28 K10:K28">
-    <cfRule type="expression" dxfId="71" priority="72">
+    <cfRule type="expression" dxfId="70" priority="72">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:Y24">
-    <cfRule type="expression" dxfId="70" priority="71">
+    <cfRule type="expression" dxfId="69" priority="71">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z30">
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="68" priority="70">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="expression" dxfId="68" priority="69">
+    <cfRule type="expression" dxfId="67" priority="69">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:O30">
-    <cfRule type="expression" dxfId="67" priority="68">
+    <cfRule type="expression" dxfId="66" priority="68">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:R30">
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="65" priority="67">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U30">
-    <cfRule type="expression" dxfId="65" priority="66">
+    <cfRule type="expression" dxfId="64" priority="66">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30:W30 Y30">
-    <cfRule type="expression" dxfId="64" priority="65">
+    <cfRule type="expression" dxfId="63" priority="65">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA30:AU30">
-    <cfRule type="expression" dxfId="63" priority="64">
+    <cfRule type="expression" dxfId="62" priority="64">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8:P24">
-    <cfRule type="expression" dxfId="62" priority="63">
+    <cfRule type="expression" dxfId="61" priority="63">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:T31">
-    <cfRule type="expression" dxfId="61" priority="62">
+    <cfRule type="expression" dxfId="60" priority="62">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31:AI31 AK31:AU31">
-    <cfRule type="expression" dxfId="60" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U31">
-    <cfRule type="expression" dxfId="59" priority="60">
+    <cfRule type="expression" dxfId="58" priority="60">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31">
-    <cfRule type="expression" dxfId="58" priority="59">
+    <cfRule type="expression" dxfId="57" priority="59">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P31">
-    <cfRule type="expression" dxfId="57" priority="58">
+    <cfRule type="expression" dxfId="56" priority="58">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N31:O31">
-    <cfRule type="expression" dxfId="56" priority="57">
+    <cfRule type="expression" dxfId="55" priority="57">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q31:R31">
-    <cfRule type="expression" dxfId="55" priority="56">
+    <cfRule type="expression" dxfId="54" priority="56">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U31">
-    <cfRule type="expression" dxfId="54" priority="55">
+    <cfRule type="expression" dxfId="53" priority="55">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA31:AI31 AK31:AU31">
-    <cfRule type="expression" dxfId="53" priority="54">
+    <cfRule type="expression" dxfId="52" priority="54">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8:AK24">
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="51" priority="53">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL8:AL24">
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="50" priority="52">
       <formula>$L8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M30:T30">
-    <cfRule type="expression" dxfId="50" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z30:AU30">
-    <cfRule type="expression" dxfId="49" priority="50">
+    <cfRule type="expression" dxfId="48" priority="50">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U30">
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="47" priority="49">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30:W30 Y30">
-    <cfRule type="expression" dxfId="47" priority="48">
+    <cfRule type="expression" dxfId="46" priority="48">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z30">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="45" priority="47">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P30">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="44" priority="46">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:O30">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="43" priority="45">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q30:R30">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="42" priority="44">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U30">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V30:W30 Y30">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="40" priority="42">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA30:AU30">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M31:T31">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="38" priority="40">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31:AI31 AK31:AU31">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U31">
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="34" priority="36">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="33" priority="35">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V31">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W31">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W31">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="30" priority="32">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W31">
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y31">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y31">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y31">
-    <cfRule type="expression" dxfId="27" priority="28">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V32">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V32">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V32">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V32">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W32">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W32">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W32">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y32">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y32">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y32">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X30:X32">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ31">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>$L31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ32">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$L29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:I31">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$L30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$L32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56740,10 +56780,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029B809A-9171-42FE-9E88-F881D2FAAE35}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -56764,53 +56804,53 @@
       <c r="A1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="42"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="42"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="41"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="M1" s="41"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="43" t="s">
         <v>214</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="43" t="s">
         <v>215</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="46" t="s">
+      <c r="I2" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="J2" s="47"/>
+      <c r="J2" s="48"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="44" t="s">
         <v>214</v>
       </c>
     </row>
@@ -56818,61 +56858,61 @@
       <c r="A3" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="42"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="44"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="45"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="43" t="s">
         <v>218</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="45"/>
+      <c r="G4" s="43" t="s">
         <v>214</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="43" t="s">
         <v>214</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="M4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="42"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="45"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="46"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
@@ -56994,16 +57034,63 @@
         <v>234</v>
       </c>
     </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="I2:J3"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G5"/>
@@ -57013,6 +57100,14 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="I2:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -57020,12 +57115,157 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="4c8003be-eb40-4e61-8d37-b1ac91d63543">
+      <UserInfo>
+        <DisplayName>Jooyeon Hwang</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hunsoo Yoo</DisplayName>
+        <AccountId>136</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jihoon Kim</DisplayName>
+        <AccountId>68</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Joowon Hong</DisplayName>
+        <AccountId>91</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dukyoung Jang</DisplayName>
+        <AccountId>69</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jonghyeok Park</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Wonwoong Yang</DisplayName>
+        <AccountId>40</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Moonyoul Lee</DisplayName>
+        <AccountId>35</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sunghwan Park</DisplayName>
+        <AccountId>52</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MuHwan Oh</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kyochul Yoon</DisplayName>
+        <AccountId>9</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Junejung Lee</DisplayName>
+        <AccountId>51</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Changdo Kim</DisplayName>
+        <AccountId>42</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jinsu Yang</DisplayName>
+        <AccountId>90</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Donghyeon Kim</DisplayName>
+        <AccountId>48</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Moogun Ahn</DisplayName>
+        <AccountId>41</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>YoungRim Lee</DisplayName>
+        <AccountId>44</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jaehun Jung</DisplayName>
+        <AccountId>64</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hasick Lim</DisplayName>
+        <AccountId>60</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jonathan Lee</DisplayName>
+        <AccountId>194</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kideuk Kwon</DisplayName>
+        <AccountId>39</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>David Rhee</DisplayName>
+        <AccountId>139</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jihoon Lee</DisplayName>
+        <AccountId>25</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Myeongsuk Song</DisplayName>
+        <AccountId>29</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sungkwan On</DisplayName>
+        <AccountId>110</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Woojin Jang</DisplayName>
+        <AccountId>104</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Wonjong Choi</DisplayName>
+        <AccountId>33</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Chihoon Park</DisplayName>
+        <AccountId>196</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Il Choi</DisplayName>
+        <AccountId>59</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57226,163 +57466,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="4c8003be-eb40-4e61-8d37-b1ac91d63543">
-      <UserInfo>
-        <DisplayName>Jooyeon Hwang</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hunsoo Yoo</DisplayName>
-        <AccountId>136</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jihoon Kim</DisplayName>
-        <AccountId>68</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Joowon Hong</DisplayName>
-        <AccountId>91</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dukyoung Jang</DisplayName>
-        <AccountId>69</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jonghyeok Park</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Wonwoong Yang</DisplayName>
-        <AccountId>40</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Moonyoul Lee</DisplayName>
-        <AccountId>35</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sunghwan Park</DisplayName>
-        <AccountId>52</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MuHwan Oh</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kyochul Yoon</DisplayName>
-        <AccountId>9</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Junejung Lee</DisplayName>
-        <AccountId>51</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Changdo Kim</DisplayName>
-        <AccountId>42</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jinsu Yang</DisplayName>
-        <AccountId>90</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Donghyeon Kim</DisplayName>
-        <AccountId>48</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Moogun Ahn</DisplayName>
-        <AccountId>41</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>YoungRim Lee</DisplayName>
-        <AccountId>44</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jaehun Jung</DisplayName>
-        <AccountId>64</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hasick Lim</DisplayName>
-        <AccountId>60</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jonathan Lee</DisplayName>
-        <AccountId>194</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kideuk Kwon</DisplayName>
-        <AccountId>39</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>David Rhee</DisplayName>
-        <AccountId>139</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jihoon Lee</DisplayName>
-        <AccountId>25</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Myeongsuk Song</DisplayName>
-        <AccountId>29</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sungkwan On</DisplayName>
-        <AccountId>110</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Woojin Jang</DisplayName>
-        <AccountId>104</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Wonjong Choi</DisplayName>
-        <AccountId>33</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Chihoon Park</DisplayName>
-        <AccountId>196</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Il Choi</DisplayName>
-        <AccountId>59</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1CE0234-F751-4660-AF32-B48DFBA9CF73}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA173A41-9F56-482D-A753-2B7D576971A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="25c2515b-9503-4120-8a04-e13f573a2b2a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4c8003be-eb40-4e61-8d37-b1ac91d63543"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -57407,18 +57511,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA173A41-9F56-482D-A753-2B7D576971A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1CE0234-F751-4660-AF32-B48DFBA9CF73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="25c2515b-9503-4120-8a04-e13f573a2b2a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="4c8003be-eb40-4e61-8d37-b1ac91d63543"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>